<commit_message>
all the options have now been implemented, buy and sell have been streamlined and fixed
</commit_message>
<xml_diff>
--- a/transaction-history.xlsx
+++ b/transaction-history.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Transactions" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
     <t xml:space="preserve">Buying transactions</t>
   </si>
@@ -71,16 +71,22 @@
     <t xml:space="preserve">orange juice</t>
   </si>
   <si>
-    <t xml:space="preserve">car</t>
-  </si>
-  <si>
-    <t xml:space="preserve">99</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19.62</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2229.72</t>
+    <t xml:space="preserve">20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Car</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1233</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123123</t>
   </si>
 </sst>
 </file>
@@ -322,11 +328,11 @@
   </sheetPr>
   <dimension ref="A1:T73"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R6" activeCellId="0" sqref="R6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T13" activeCellId="0" sqref="T13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.94140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10"/>
@@ -497,11 +503,11 @@
   </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.86"/>
@@ -542,29 +548,33 @@
       <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>123</v>
-      </c>
-      <c r="F3" s="1" t="n">
-        <v>1000</v>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Everything now mostly works and its usable, still working on making an overview sheet
</commit_message>
<xml_diff>
--- a/transaction-history.xlsx
+++ b/transaction-history.xlsx
@@ -10,6 +10,7 @@
   <sheets>
     <sheet name="Transactions" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Inventory" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Overview" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
   <si>
     <t xml:space="preserve">Buying transactions</t>
   </si>
@@ -57,36 +58,6 @@
   </si>
   <si>
     <t xml:space="preserve">Inventory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 pound fish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">orange juice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Car</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1233</t>
-  </si>
-  <si>
-    <t xml:space="preserve">123123</t>
   </si>
 </sst>
 </file>
@@ -96,7 +67,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -118,6 +89,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -209,15 +186,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -245,7 +222,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -326,13 +303,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T73"/>
+  <dimension ref="A1:AF73"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T13" activeCellId="0" sqref="T13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P19" activeCellId="0" sqref="P19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.94140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10"/>
@@ -340,19 +317,20 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="12.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="2" width="13.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="21.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="12.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="18.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="13.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="3" width="14.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="13.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="25.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="4" width="12.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="4" width="18.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="4" width="12.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="4" width="13.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="4" width="14.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="4" width="15.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="21" style="1" width="8.94"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -407,6 +385,17 @@
       <c r="T1" s="8" t="s">
         <v>7</v>
       </c>
+      <c r="V1" s="0"/>
+      <c r="W1" s="0"/>
+      <c r="X1" s="0"/>
+      <c r="Y1" s="0"/>
+      <c r="Z1" s="0"/>
+      <c r="AA1" s="0"/>
+      <c r="AB1" s="0"/>
+      <c r="AC1" s="0"/>
+      <c r="AD1" s="0"/>
+      <c r="AE1" s="0"/>
+      <c r="AF1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
@@ -501,16 +490,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
+      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="1" width="11.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="11.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="15.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="23.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="11" style="1" width="11.77"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -531,56 +525,12 @@
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -590,4 +540,41 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="M1:M6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L27" activeCellId="0" sqref="L27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="12.9"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="M6" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10 &amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10 &amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>